<commit_message>
updated data and analyses
</commit_message>
<xml_diff>
--- a/data/conversion or recalculation of effect sizes/effect size conversion formulae and workings.xlsx
+++ b/data/conversion or recalculation of effect sizes/effect size conversion formulae and workings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/reanalysis-of-vahey-2015/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/reanalysis-of-vahey-2015/data/conversion or recalculation of effect sizes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7400C9F-CD26-AE41-9F2F-483040ED73FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D2E868-01DC-B542-B4F3-967C46DC3E8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="144">
-  <si>
-    <t>Hooper, Villatte,  Neofotistou &amp; McHugh (2010)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="139">
   <si>
     <t>Nicholson &amp; Barnes-Holmes (2012a)</t>
   </si>
@@ -37,9 +34,6 @@
     <t>Parling, Cernvall, Stewart, Barnes-Holmes &amp; Ghaderi (2011)</t>
   </si>
   <si>
-    <t>Compound DIRAP for all four IRAP trial-types about experiential avoidance</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -191,15 +185,6 @@
   </si>
   <si>
     <t>correlation</t>
-  </si>
-  <si>
-    <t>mindfulness group</t>
-  </si>
-  <si>
-    <t>Hooper et al., 2010</t>
-  </si>
-  <si>
-    <t>F(1, 22) = 5.37, ηp2 = .196, therefore r = .44</t>
   </si>
   <si>
     <t>Hussey &amp; Barnes-Holmes, 2012</t>
@@ -2508,8 +2493,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:L191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2519,22 +2504,22 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2542,12 +2527,12 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2555,30 +2540,30 @@
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="10">
         <v>0.23100000000000001</v>
@@ -2599,7 +2584,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="11">
         <v>-0.03</v>
@@ -2625,7 +2610,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="11">
         <v>-0.18</v>
@@ -2646,7 +2631,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="11">
         <v>-0.12</v>
@@ -2664,36 +2649,36 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2"/>
       <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24">
         <v>-0.05</v>
@@ -2715,10 +2700,10 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
         <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
       </c>
       <c r="C25">
         <v>0.34</v>
@@ -2742,10 +2727,10 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
         <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
       </c>
       <c r="C27" s="11">
         <v>-0.22</v>
@@ -2767,10 +2752,10 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="11">
         <v>0.1</v>
@@ -2786,33 +2771,33 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2"/>
       <c r="C35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="G35" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11">
@@ -2827,7 +2812,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11">
@@ -2844,7 +2829,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -2861,7 +2846,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -2873,7 +2858,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
@@ -2890,7 +2875,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
@@ -2902,20 +2887,20 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="B46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B47">
         <v>15</v>
@@ -2926,7 +2911,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B48">
         <v>5</v>
@@ -2934,7 +2919,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B49">
         <v>8</v>
@@ -2942,7 +2927,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B50">
         <v>0.41499999999999998</v>
@@ -2953,7 +2938,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B51">
         <v>0.21438441999999999</v>
@@ -2964,17 +2949,17 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2985,19 +2970,19 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F59" s="6">
         <v>0.41</v>
@@ -3008,25 +2993,25 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K59" s="4"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F60" s="16">
         <v>0.27739999999999998</v>
@@ -3037,25 +3022,25 @@
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="J60" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K60" s="4"/>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F61" s="16">
         <v>0.27739999999999998</v>
@@ -3066,25 +3051,25 @@
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K61" s="4"/>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F62" s="16">
         <v>0.27739999999999998</v>
@@ -3095,25 +3080,25 @@
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="J62" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K62" s="4"/>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F63" s="16">
         <v>0.27739999999999998</v>
@@ -3124,21 +3109,21 @@
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="J63" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K63" s="4"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="5"/>
       <c r="D64" s="28" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E64" s="28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F64" s="28">
         <v>8.4000000000000005E-2</v>
@@ -3153,15 +3138,15 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
       <c r="D65" s="28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F65" s="28">
         <v>8.7999999999999995E-2</v>
@@ -3176,15 +3161,15 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="5"/>
       <c r="D66" s="28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F66" s="28">
         <v>0.214</v>
@@ -3199,15 +3184,15 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="5"/>
       <c r="D67" s="28" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F67" s="28">
         <v>0.18099999999999999</v>
@@ -3222,15 +3207,15 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="5"/>
       <c r="D68" s="28" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E68" s="28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F68" s="28">
         <v>0.20499999999999999</v>
@@ -3245,15 +3230,15 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="5"/>
       <c r="D69" s="28" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F69" s="28">
         <v>0.255</v>
@@ -3268,15 +3253,15 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="5"/>
       <c r="D70" s="28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E70" s="28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F70" s="28">
         <v>3.5999999999999997E-2</v>
@@ -3291,15 +3276,15 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="5"/>
       <c r="D71" s="28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E71" s="28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F71" s="28">
         <v>0.16900000000000001</v>
@@ -3314,15 +3299,15 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="5"/>
       <c r="D72" s="28" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E72" s="28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F72" s="28">
         <v>0.21099999999999999</v>
@@ -3337,15 +3322,15 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="5"/>
       <c r="D73" s="28" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E73" s="28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F73" s="28">
         <v>0.22900000000000001</v>
@@ -3359,68 +3344,48 @@
       <c r="K73" s="4"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="A76" s="20"/>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="17" t="s">
-        <v>51</v>
-      </c>
+      <c r="A77" s="17"/>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F79" s="4">
-        <v>0.44</v>
-      </c>
-      <c r="G79" s="4">
-        <v>22</v>
-      </c>
+      <c r="A79" s="4"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
       <c r="H79" s="4"/>
-      <c r="I79" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="I79" s="4"/>
       <c r="J79" s="5"/>
       <c r="K79" s="4"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="20" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="C85" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C86" s="6">
         <v>0.156</v>
@@ -3431,10 +3396,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C87" s="6">
         <v>0.14599999999999999</v>
@@ -3445,10 +3410,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C88" s="6">
         <v>-2.9000000000000001E-2</v>
@@ -3459,10 +3424,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C89" s="6">
         <v>-8.2000000000000003E-2</v>
@@ -3473,10 +3438,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C90" s="6">
         <v>5.1999999999999998E-2</v>
@@ -3487,10 +3452,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C91" s="6">
         <v>-6.8000000000000005E-2</v>
@@ -3501,10 +3466,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C92" s="6">
         <v>4.2000000000000003E-2</v>
@@ -3515,10 +3480,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C93" s="6">
         <v>0.14799999999999999</v>
@@ -3529,10 +3494,10 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B94" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C94" s="6">
         <v>0.38700000000000001</v>
@@ -3543,10 +3508,10 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B95" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C95" s="6">
         <v>0.161</v>
@@ -3557,10 +3522,10 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B96" s="23" t="s">
         <v>119</v>
-      </c>
-      <c r="B96" s="23" t="s">
-        <v>124</v>
       </c>
       <c r="C96" s="6">
         <v>-0.19400000000000001</v>
@@ -3571,10 +3536,10 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B97" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C97" s="6">
         <v>-9.8000000000000004E-2</v>
@@ -3585,10 +3550,10 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B98" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C98" s="6">
         <v>0.16900000000000001</v>
@@ -3599,10 +3564,10 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B99" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C99" s="6">
         <v>0.40500000000000003</v>
@@ -3613,10 +3578,10 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B100" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C100" s="6">
         <v>0.11</v>
@@ -3627,10 +3592,10 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B101" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C101" s="6">
         <v>0.28999999999999998</v>
@@ -3641,10 +3606,10 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B102" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C102" s="6">
         <v>0.17599999999999999</v>
@@ -3655,10 +3620,10 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B103" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C103" s="6">
         <v>-5.8000000000000003E-2</v>
@@ -3669,10 +3634,10 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B104" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C104" s="6">
         <v>0.157</v>
@@ -3683,10 +3648,10 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C105" s="6">
         <v>0.161</v>
@@ -3697,10 +3662,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C106" s="6">
         <v>-5.2999999999999999E-2</v>
@@ -3711,10 +3676,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C107" s="6">
         <v>8.3000000000000004E-2</v>
@@ -3725,10 +3690,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C108" s="6">
         <v>-6.8000000000000005E-2</v>
@@ -3739,10 +3704,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C109" s="6">
         <v>0.254</v>
@@ -3753,10 +3718,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C110" s="6">
         <v>7.1999999999999995E-2</v>
@@ -3767,10 +3732,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C111" s="6">
         <v>-0.29499999999999998</v>
@@ -3781,10 +3746,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="23" t="s">
         <v>120</v>
-      </c>
-      <c r="B112" s="23" t="s">
-        <v>125</v>
       </c>
       <c r="C112" s="6">
         <v>-8.2000000000000003E-2</v>
@@ -3795,10 +3760,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C113" s="6">
         <v>2E-3</v>
@@ -3809,10 +3774,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B114" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C114" s="6">
         <v>5.2999999999999999E-2</v>
@@ -3823,10 +3788,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B115" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C115" s="6">
         <v>-0.13500000000000001</v>
@@ -3837,10 +3802,10 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B116" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C116" s="23">
         <v>0.10100000000000001</v>
@@ -3851,10 +3816,10 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B117" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C117" s="23">
         <v>-3.5000000000000003E-2</v>
@@ -3865,10 +3830,10 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B118" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C118" s="23">
         <v>-0.112</v>
@@ -3879,10 +3844,10 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B119" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C119" s="23">
         <v>2.4E-2</v>
@@ -3893,10 +3858,10 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B120" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C120" s="23">
         <v>-0.02</v>
@@ -3907,10 +3872,10 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B121" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C121" s="23">
         <v>0.20200000000000001</v>
@@ -3921,10 +3886,10 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B122" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C122" s="23">
         <v>1.4999999999999999E-2</v>
@@ -3935,10 +3900,10 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B123" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C123" s="23">
         <v>-6.0999999999999999E-2</v>
@@ -3949,10 +3914,10 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B124" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C124" s="23">
         <v>0.193</v>
@@ -3963,10 +3928,10 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B125" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C125" s="23">
         <v>0.11</v>
@@ -3977,10 +3942,10 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B126" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C126" s="23">
         <v>9.6000000000000002E-2</v>
@@ -3991,10 +3956,10 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B127" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C127" s="23">
         <v>5.1999999999999998E-2</v>
@@ -4005,10 +3970,10 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B128" s="23" t="s">
         <v>121</v>
-      </c>
-      <c r="B128" s="23" t="s">
-        <v>126</v>
       </c>
       <c r="C128" s="23">
         <v>6.9000000000000006E-2</v>
@@ -4019,10 +3984,10 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B129" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C129" s="23">
         <v>0.13700000000000001</v>
@@ -4033,10 +3998,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B130" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C130" s="23">
         <v>0.13900000000000001</v>
@@ -4047,10 +4012,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B131" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C131" s="23">
         <v>-0.34300000000000003</v>
@@ -4061,10 +4026,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B132" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C132" s="23">
         <v>-0.19700000000000001</v>
@@ -4075,10 +4040,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B133" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C133" s="23">
         <v>-4.4999999999999998E-2</v>
@@ -4089,10 +4054,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B134" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C134" s="23">
         <v>-8.1000000000000003E-2</v>
@@ -4103,10 +4068,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B135" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C135" s="23">
         <v>-0.19600000000000001</v>
@@ -4117,10 +4082,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B136" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C136" s="23">
         <v>0.13600000000000001</v>
@@ -4131,10 +4096,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B137" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C137" s="23">
         <v>2.5999999999999999E-2</v>
@@ -4145,10 +4110,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B138" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C138" s="23">
         <v>6.2E-2</v>
@@ -4159,10 +4124,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B139" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C139" s="23">
         <v>-0.32100000000000001</v>
@@ -4173,10 +4138,10 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B140" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C140" s="23">
         <v>-1.7999999999999999E-2</v>
@@ -4187,10 +4152,10 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B141" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C141" s="23">
         <v>0.41599999999999998</v>
@@ -4201,10 +4166,10 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B142" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C142" s="23">
         <v>0.22800000000000001</v>
@@ -4215,10 +4180,10 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B143" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C143" s="23">
         <v>0.107</v>
@@ -4229,10 +4194,10 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C144" s="23">
         <v>-0.185</v>
@@ -4243,10 +4208,10 @@
     </row>
     <row r="145" spans="1:11">
       <c r="A145" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C145" s="23">
         <v>0.23499999999999999</v>
@@ -4257,29 +4222,29 @@
     </row>
     <row r="148" spans="1:11">
       <c r="A148" s="21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="149" spans="1:11">
       <c r="A149" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="151" spans="1:11">
       <c r="A151" s="22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C151" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F151" s="4">
         <v>0.42499999999999999</v>
@@ -4288,24 +4253,24 @@
         <v>28</v>
       </c>
       <c r="I151" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="152" spans="1:11" s="4" customFormat="1">
       <c r="A152" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F152" s="4">
         <v>0.47</v>
@@ -4314,25 +4279,25 @@
         <v>28</v>
       </c>
       <c r="I152" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K152" s="5"/>
     </row>
     <row r="153" spans="1:11">
       <c r="A153" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F153" s="4">
         <v>0.24</v>
@@ -4341,24 +4306,24 @@
         <v>28</v>
       </c>
       <c r="I153" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="154" spans="1:11">
       <c r="A154" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F154" s="4">
         <v>0.11</v>
@@ -4367,24 +4332,24 @@
         <v>28</v>
       </c>
       <c r="I154" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="155" spans="1:11">
       <c r="A155" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F155" s="4">
         <v>0.05</v>
@@ -4393,24 +4358,24 @@
         <v>25</v>
       </c>
       <c r="I155" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="156" spans="1:11">
       <c r="A156" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F156" s="4">
         <v>0.3</v>
@@ -4419,24 +4384,24 @@
         <v>25</v>
       </c>
       <c r="I156" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="157" spans="1:11">
       <c r="A157" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F157" s="4">
         <v>0.05</v>
@@ -4445,24 +4410,24 @@
         <v>25</v>
       </c>
       <c r="I157" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="158" spans="1:11">
       <c r="A158" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F158" s="4">
         <v>0.31</v>
@@ -4471,24 +4436,24 @@
         <v>25</v>
       </c>
       <c r="I158" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="159" spans="1:11">
       <c r="A159" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F159" s="4">
         <v>0.37</v>
@@ -4497,24 +4462,24 @@
         <v>30</v>
       </c>
       <c r="I159" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="160" spans="1:11">
       <c r="A160" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F160" s="4">
         <v>0.06</v>
@@ -4523,24 +4488,24 @@
         <v>30</v>
       </c>
       <c r="I160" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="161" spans="1:12">
       <c r="A161" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F161" s="4">
         <v>0.27</v>
@@ -4549,24 +4514,24 @@
         <v>30</v>
       </c>
       <c r="I161" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="162" spans="1:12">
       <c r="A162" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F162" s="4">
         <v>0.02</v>
@@ -4575,24 +4540,24 @@
         <v>30</v>
       </c>
       <c r="I162" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="163" spans="1:12">
       <c r="A163" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F163" s="4">
         <v>0.12</v>
@@ -4601,24 +4566,24 @@
         <v>27</v>
       </c>
       <c r="I163" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="164" spans="1:12">
       <c r="A164" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F164" s="4">
         <v>0.2</v>
@@ -4627,24 +4592,24 @@
         <v>27</v>
       </c>
       <c r="I164" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="165" spans="1:12">
       <c r="A165" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F165" s="4">
         <v>0.08</v>
@@ -4653,24 +4618,24 @@
         <v>27</v>
       </c>
       <c r="I165" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="166" spans="1:12">
       <c r="A166" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F166" s="4">
         <v>0.34</v>
@@ -4679,64 +4644,64 @@
         <v>27</v>
       </c>
       <c r="I166" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="168" spans="1:12">
       <c r="A168" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L168" s="24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="170" spans="1:12">
       <c r="A170" s="21" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="171" spans="1:12">
       <c r="A171" s="17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="172" spans="1:12">
       <c r="A172" s="17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="173" spans="1:12">
       <c r="D173" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F173" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H173" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I173" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L173" s="25"/>
     </row>
     <row r="174" spans="1:12">
       <c r="A174" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
       <c r="D174" t="s">
+        <v>11</v>
+      </c>
+      <c r="E174" t="s">
         <v>13</v>
       </c>
-      <c r="E174" t="s">
-        <v>15</v>
-      </c>
       <c r="F174" t="s">
+        <v>11</v>
+      </c>
+      <c r="G174" t="s">
         <v>13</v>
-      </c>
-      <c r="G174" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="175" spans="1:12">
@@ -4774,7 +4739,7 @@
     </row>
     <row r="178" spans="1:8">
       <c r="A178" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
@@ -4786,45 +4751,45 @@
     </row>
     <row r="180" spans="1:8">
       <c r="A180" s="21" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
     </row>
     <row r="181" spans="1:8">
       <c r="B181" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C181" t="s">
+        <v>131</v>
+      </c>
+      <c r="E181" t="s">
+        <v>135</v>
+      </c>
+      <c r="F181" t="s">
+        <v>7</v>
+      </c>
+      <c r="G181" t="s">
         <v>136</v>
       </c>
-      <c r="E181" t="s">
-        <v>140</v>
-      </c>
-      <c r="F181" t="s">
-        <v>9</v>
-      </c>
-      <c r="G181" t="s">
-        <v>141</v>
-      </c>
       <c r="H181" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="182" spans="1:8">
       <c r="C182" t="s">
+        <v>11</v>
+      </c>
+      <c r="D182" t="s">
         <v>13</v>
-      </c>
-      <c r="D182" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="183" spans="1:8">
       <c r="A183" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B183" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C183">
         <v>0.45</v>
@@ -4848,10 +4813,10 @@
     </row>
     <row r="184" spans="1:8">
       <c r="A184" t="s">
+        <v>129</v>
+      </c>
+      <c r="B184" t="s">
         <v>134</v>
-      </c>
-      <c r="B184" t="s">
-        <v>139</v>
       </c>
       <c r="C184">
         <v>0.12</v>
@@ -4869,10 +4834,10 @@
     </row>
     <row r="185" spans="1:8">
       <c r="A185" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B185" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C185">
         <v>0.16</v>
@@ -4896,10 +4861,10 @@
     </row>
     <row r="186" spans="1:8">
       <c r="A186" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B186" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C186">
         <v>0.35</v>
@@ -4917,10 +4882,10 @@
     </row>
     <row r="188" spans="1:8">
       <c r="A188" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B188" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C188">
         <v>0.5</v>
@@ -4928,10 +4893,10 @@
     </row>
     <row r="189" spans="1:8">
       <c r="A189" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B189" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C189">
         <v>0.19</v>
@@ -4939,10 +4904,10 @@
     </row>
     <row r="190" spans="1:8">
       <c r="A190" t="s">
+        <v>129</v>
+      </c>
+      <c r="B190" t="s">
         <v>134</v>
-      </c>
-      <c r="B190" t="s">
-        <v>139</v>
       </c>
       <c r="C190">
         <v>0.14000000000000001</v>
@@ -4950,10 +4915,10 @@
     </row>
     <row r="191" spans="1:8">
       <c r="A191" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B191" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C191">
         <v>0.37</v>
@@ -4963,10 +4928,9 @@
   <hyperlinks>
     <hyperlink ref="A55" r:id="rId1" location="transform2" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
     <hyperlink ref="A56" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="A77" r:id="rId3" location="transform2" display="https://www.psychometrica.de/effect_size.html - transform2" xr:uid="{CB1F8952-EAAF-5043-B32C-45793F40689D}"/>
-    <hyperlink ref="A149" r:id="rId4" location="transform2" display="https://www.psychometrica.de/effect_size.html - transform2" xr:uid="{756CA905-2492-7243-BDE6-919B0A972D19}"/>
-    <hyperlink ref="A171" r:id="rId5" xr:uid="{E2E502B4-57DA-CD42-8DA9-5DF9A52BB20C}"/>
-    <hyperlink ref="A172" r:id="rId6" xr:uid="{5E55FEFE-0882-9641-924F-87ECCFB51070}"/>
+    <hyperlink ref="A149" r:id="rId3" location="transform2" display="https://www.psychometrica.de/effect_size.html - transform2" xr:uid="{756CA905-2492-7243-BDE6-919B0A972D19}"/>
+    <hyperlink ref="A171" r:id="rId4" xr:uid="{E2E502B4-57DA-CD42-8DA9-5DF9A52BB20C}"/>
+    <hyperlink ref="A172" r:id="rId5" xr:uid="{5E55FEFE-0882-9641-924F-87ECCFB51070}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4994,19 +4958,19 @@
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F1" s="18">
         <v>0.27739999999999998</v>
@@ -5017,33 +4981,33 @@
         <v>32</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K1" s="19" t="b">
         <v>0</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F2" s="18">
         <v>0.27739999999999998</v>
@@ -5054,33 +5018,33 @@
         <v>32</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K2" s="19" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="4" customFormat="1">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F3" s="18">
         <v>0.27739999999999998</v>
@@ -5091,33 +5055,33 @@
         <v>32</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K3" s="19" t="b">
         <v>0</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="4" customFormat="1">
       <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F4" s="18">
         <v>0.27739999999999998</v>
@@ -5128,33 +5092,33 @@
         <v>32</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K4" s="19" t="b">
         <v>0</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="4" customFormat="1">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="27">
@@ -5167,34 +5131,34 @@
         <v>27</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K5" s="19" t="b">
         <v>0</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="1" customFormat="1">
       <c r="A8" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G8" s="30" t="b">
         <v>0</v>
@@ -5230,25 +5194,25 @@
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1">
       <c r="A9" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G9" s="30" t="b">
         <v>0</v>
@@ -5284,7 +5248,7 @@
       </c>
       <c r="R9" s="6"/>
       <c r="S9" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>